<commit_message>
Fix Plots.xlsx data names
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B960C6-DEE3-4CBB-AB02-1CAE12D3BC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431C8A4D-8AA9-48E1-9B1A-211F2330CE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="35010" windowHeight="18285" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>yValuesLimits</t>
   </si>
   <si>
-    <t>Laskin 1982.Group A_Aciclovir_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
-  </si>
-  <si>
     <t>P4</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>nsd</t>
+  </si>
+  <si>
+    <t>Laskin 1982.Group A_Aciclovir_1_Human__PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
   </si>
 </sst>
 </file>
@@ -282,9 +282,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -322,7 +322,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -428,7 +428,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -570,7 +570,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -581,8 +581,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
         <v>39</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -698,13 +698,13 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -724,10 +724,10 @@
         <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -762,7 +762,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -819,7 +819,7 @@
         <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s">
         <v>42</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -884,7 +884,7 @@
         <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M5">
         <v>1.96</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1079,6 +1079,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1281,27 +1301,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1318,23 +1337,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Fixed observed data naming (`MALE`)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431C8A4D-8AA9-48E1-9B1A-211F2330CE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0A8FCC-2592-450E-9B2B-BD46DC2D9EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="35010" windowHeight="18285" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="35010" windowHeight="18285" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -220,7 +220,7 @@
     <t>nsd</t>
   </si>
   <si>
-    <t>Laskin 1982.Group A_Aciclovir_1_Human__PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
+    <t>Laskin 1982.Group A_Aciclovir_1_Human_MALE_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
   </si>
 </sst>
 </file>
@@ -1079,26 +1079,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1301,26 +1281,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1337,4 +1318,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Importer config grouping (#779)
* - The Importer configuration provided with the template project has been
  updated to include `Gender` in the naming pattern

- Importer configuration created with release version of OSPS

* Increase version

* Fix Plots.xlsx data names

* - Fixed observed data naming (`MALE`)

* Add a test for loadObservedData using default esqlabs importer Configuration

---------

Co-authored-by: Felix MIL <dev@felixmil.com>
Co-authored-by: Felix MIL <34234913+Felixmil@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B960C6-DEE3-4CBB-AB02-1CAE12D3BC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0A8FCC-2592-450E-9B2B-BD46DC2D9EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="35010" windowHeight="18285" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>yValuesLimits</t>
   </si>
   <si>
-    <t>Laskin 1982.Group A_Aciclovir_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
-  </si>
-  <si>
     <t>P4</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>nsd</t>
+  </si>
+  <si>
+    <t>Laskin 1982.Group A_Aciclovir_1_Human_MALE_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
   </si>
 </sst>
 </file>
@@ -282,9 +282,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -322,7 +322,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -428,7 +428,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -570,7 +570,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -581,8 +581,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
         <v>39</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -698,13 +698,13 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -724,10 +724,10 @@
         <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -762,7 +762,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -819,7 +819,7 @@
         <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s">
         <v>42</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -884,7 +884,7 @@
         <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M5">
         <v>1.96</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added title and subtitle to exemplary plot configuration and plot grid - Fixes plot subtitle not added to plot configuration
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0A8FCC-2592-450E-9B2B-BD46DC2D9EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FB839A-93D5-46E9-9467-F865FBA2C3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="35010" windowHeight="18285" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>group</t>
   </si>
@@ -221,6 +221,21 @@
   </si>
   <si>
     <t>Laskin 1982.Group A_Aciclovir_1_Human_MALE_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>PlotTitle</t>
+  </si>
+  <si>
+    <t>PlotSubtitle</t>
+  </si>
+  <si>
+    <t>GridTitle</t>
+  </si>
+  <si>
+    <t>GridSubtitle</t>
   </si>
 </sst>
 </file>
@@ -581,22 +596,22 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.3046875" customWidth="1"/>
+    <col min="7" max="7" width="24.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -637,7 +652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -664,7 +679,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -687,7 +702,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -713,7 +728,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -760,28 +775,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B8908D-615D-4618-BFCF-D7DBA10892F0}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.3046875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.3046875" customWidth="1"/>
+    <col min="14" max="14" width="12.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -824,8 +839,11 @@
       <c r="N1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -835,14 +853,20 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
       <c r="E2" t="s">
         <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -856,7 +880,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -867,7 +891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -910,15 +934,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3CB29-E548-4DAF-A68B-014C6C094FDA}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -928,16 +952,25 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -945,7 +978,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -966,14 +999,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -998,19 +1031,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1029,34 +1062,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1072,13 +1105,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1281,15 +1323,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1302,6 +1335,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1320,14 +1361,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>

</xml_diff>